<commit_message>
Update query for checking users with their google account
</commit_message>
<xml_diff>
--- a/server/references/Team List for Peer Feedback 2023Q2.xlsx
+++ b/server/references/Team List for Peer Feedback 2023Q2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atxdefense/jsProjects/excelExtractor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atxdefense/jsProjects/codeTester/template/server/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF4D560-B7F1-944A-8E2A-2AB2CB075A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F412CC9-8CB2-4D44-9D75-B629B75D6AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="534">
   <si>
     <t>Name</t>
   </si>
@@ -1626,6 +1626,18 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>automation_do_no_respond</t>
+  </si>
+  <si>
+    <t>cohort 23</t>
+  </si>
+  <si>
+    <t>SDU 4</t>
+  </si>
+  <si>
+    <t>automation_do_not_respond.mil@swf.army.mil</t>
   </si>
 </sst>
 </file>
@@ -1689,12 +1701,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1913,10 +1926,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3543,6 +3556,23 @@
       <c r="E90" s="2" t="str">
         <f>VLOOKUP(A90,Emails!A:D,4,FALSE)</f>
         <v>ryan.c.miller94.mil@swf.army.mil</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>